<commit_message>
include addtionalDataUnique.xslx into the rawToJSON.py conversion, additionalDataUnique.xlsx updated and json regenerated
</commit_message>
<xml_diff>
--- a/data_preparation/additionalDataUnique.xlsx
+++ b/data_preparation/additionalDataUnique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duke\2021REU\nanomineParser\data_preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8461A4FA-CDF1-477A-B633-542CEC174022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6AD109-89E9-40E7-AF9A-1C8522CEEF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25490" yWindow="-200" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="45">
   <si>
     <t>file</t>
   </si>
@@ -85,6 +85,90 @@
   </si>
   <si>
     <t>yUnitType</t>
+  </si>
+  <si>
+    <t>10^6 Hz</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>*10^3Hz</t>
+  </si>
+  <si>
+    <t>*10^6 Hz</t>
+  </si>
+  <si>
+    <t>kHz</t>
+  </si>
+  <si>
+    <t>1000 Hz</t>
+  </si>
+  <si>
+    <t>1000000 Hz</t>
+  </si>
+  <si>
+    <t>*10^9 Hz</t>
+  </si>
+  <si>
+    <t>1000000000 Hz</t>
+  </si>
+  <si>
+    <t>GHz</t>
+  </si>
+  <si>
+    <t>rad/second</t>
+  </si>
+  <si>
+    <t>rad*s^{-1}</t>
+  </si>
+  <si>
+    <t>Pascal</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>1000 Pa</t>
+  </si>
+  <si>
+    <t>kPa</t>
+  </si>
+  <si>
+    <t>1000 Pascal</t>
+  </si>
+  <si>
+    <t>*10^3 Pa</t>
+  </si>
+  <si>
+    <t>1000000 Pa</t>
+  </si>
+  <si>
+    <t>1000000 Pascal</t>
+  </si>
+  <si>
+    <t>*10^6 Pa</t>
+  </si>
+  <si>
+    <t>MPa</t>
+  </si>
+  <si>
+    <t>1000000000 Pa</t>
+  </si>
+  <si>
+    <t>1000000000 Pascal</t>
+  </si>
+  <si>
+    <t>*10^9 Pa</t>
+  </si>
+  <si>
+    <t>GPa</t>
   </si>
 </sst>
 </file>
@@ -930,10 +1014,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q380"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" sqref="A1:Q1"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1001,6 +1085,346 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N13" t="s">
+        <v>40</v>
+      </c>
+      <c r="O13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" t="s">
+        <v>44</v>
+      </c>
+      <c r="O16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="7:15" x14ac:dyDescent="0.45">
+      <c r="G17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N17" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="7:15" x14ac:dyDescent="0.45">
+      <c r="G18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" t="s">
+        <v>43</v>
+      </c>
+      <c r="N18" t="s">
+        <v>44</v>
+      </c>
+      <c r="O18" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="379" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M379" s="1"/>
     </row>

</xml_diff>

<commit_message>
rawDataUnique update (greek letter \omega added as name for stdName Frequency
</commit_message>
<xml_diff>
--- a/data_preparation/additionalDataUnique.xlsx
+++ b/data_preparation/additionalDataUnique.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duke\2021REU\nanomineParser\data_preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6AD109-89E9-40E7-AF9A-1C8522CEEF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB86B42-CDDF-43E4-A04A-23590CB41108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-200" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1222" yWindow="-98" windowWidth="18076" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rawDataUnique" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="46">
   <si>
     <t>file</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>GPa</t>
+  </si>
+  <si>
+    <t>ω</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1020,7 @@
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1086,6 +1089,12 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
@@ -1093,6 +1102,12 @@
         <v>22</v>
       </c>
       <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" t="s">
         <v>19</v>
       </c>
       <c r="M2" t="s">

</xml_diff>